<commit_message>
Update Prefeitura de Itapema_itaitaitia.xlsx
</commit_message>
<xml_diff>
--- a/orcamentos/Prefeitura de Itapema_itaitaitia.xlsx
+++ b/orcamentos/Prefeitura de Itapema_itaitaitia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\myxlsm\orcamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8B8689-0FA2-4DF7-94CC-75B8FB53A8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234158B4-8347-480D-BEE8-520EA44B8387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,10 @@
     <sheet name="paraFilter" sheetId="6" r:id="rId2"/>
     <sheet name="resultado" sheetId="5" r:id="rId3"/>
     <sheet name="cenarios" sheetId="4" r:id="rId4"/>
-    <sheet name="Centro da Cidade" sheetId="7" r:id="rId5"/>
+    <sheet name="Centro da Cidade" sheetId="8" r:id="rId5"/>
+    <sheet name="Fundos da Cidade" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -78,67 +79,88 @@
     <t>C:\GitHub\myxlsm\orcamentos\Prefeitura de Itapema_itaitaitia.xlsx</t>
   </si>
   <si>
+    <t>Seq.</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Qtd.</t>
+  </si>
+  <si>
+    <t>Alt.</t>
+  </si>
+  <si>
+    <t>Larg.</t>
+  </si>
+  <si>
+    <t>Comp.</t>
+  </si>
+  <si>
+    <t>PotUnit</t>
+  </si>
+  <si>
+    <t>ValorUnit</t>
+  </si>
+  <si>
+    <t>Desconto</t>
+  </si>
+  <si>
+    <t>Descricao 1</t>
+  </si>
+  <si>
+    <t>Descricao 2</t>
+  </si>
+  <si>
+    <t>Descricao 3</t>
+  </si>
+  <si>
+    <t>Valor Total</t>
+  </si>
+  <si>
+    <t>AD09</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>0,5</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>Rena aramada, produzido em alumínio e pintura, com detalhes em LED. Branco</t>
+  </si>
+  <si>
+    <t>Rena aramada, medindo aproximadamente 1,10m de altura x 0,50m de largura x 1,20m de comprimento, produzido em alumínio, com pintura em esmalte sintético automotivo na cor branca e verniz automotivo brilhante com detalhes de conjuntos com 100 LEDs brancos, medindo aproximadamente 8,5m de comprimento, fio elétrico branco 2 x 0,5mm², consumo médio de 7W de potência, na tensão de 220v.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rena do papai noel aramada, tridimensional, produzida com arames de alumíno, pintura em epóxi na cor branca, aplicação de lâmpadas de LED brancas, com fio branco ou morno (medida do fio: 2x0,5mm²). Medidas das figuras: mínimo: 1,05m de altura x 0,45m de largura x 1,15m de comprimento / máximo: 1,15m de altura x 0,55m de largura x 1,25 de profundidade. </t>
+  </si>
+  <si>
+    <t>Fundos da Cidade</t>
+  </si>
+  <si>
     <t>Centro da Cidade</t>
   </si>
   <si>
-    <t>Seq.</t>
-  </si>
-  <si>
-    <t>Codigo</t>
-  </si>
-  <si>
-    <t>Qtd.</t>
-  </si>
-  <si>
-    <t>Alt.</t>
-  </si>
-  <si>
-    <t>Larg.</t>
-  </si>
-  <si>
-    <t>Comp.</t>
-  </si>
-  <si>
-    <t>PotUnit</t>
-  </si>
-  <si>
-    <t>ValorUnit</t>
-  </si>
-  <si>
-    <t>Desconto</t>
-  </si>
-  <si>
-    <t>Descricao 1</t>
-  </si>
-  <si>
-    <t>Descricao 2</t>
-  </si>
-  <si>
-    <t>Descricao 3</t>
-  </si>
-  <si>
-    <t>Valor Total</t>
-  </si>
-  <si>
-    <t>AD09</t>
-  </si>
-  <si>
-    <t>1,1</t>
-  </si>
-  <si>
-    <t>0,5</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>Rena aramada, produzido em alumínio e pintura, com detalhes em LED. Branco</t>
-  </si>
-  <si>
-    <t>Rena aramada, medindo aproximadamente 1,10m de altura x 0,50m de largura x 1,20m de comprimento, produzido em alumínio, com pintura em esmalte sintético automotivo na cor branca e verniz automotivo brilhante com detalhes de conjuntos com 100 LEDs brancos, medindo aproximadamente 8,5m de comprimento, fio elétrico branco 2 x 0,5mm², consumo médio de 7W de potência, na tensão de 220v.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rena do papai noel aramada, tridimensional, produzida com arames de alumíno, pintura em epóxi na cor branca, aplicação de lâmpadas de LED brancas, com fio branco ou morno (medida do fio: 2x0,5mm²). Medidas das figuras: mínimo: 1,05m de altura x 0,45m de largura x 1,15m de comprimento / máximo: 1,15m de altura x 0,55m de largura x 1,25 de profundidade. </t>
+    <t>AD03</t>
+  </si>
+  <si>
+    <t>0,63</t>
+  </si>
+  <si>
+    <t>0,7</t>
+  </si>
+  <si>
+    <t>Pastor e Ovelha, produzido em alumínio e pintura branca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pastor e ovelha aramados, medindo aproximadamente o Pastor 1,85m de altura x 0,65m de largura x 0,75m de comprimento e a ovelha  0,45m  de altura x 0,22m de largura e 0,75m de comprimento, produzidos em alumínio, com pintura em esmalte sintético automotivo na cor branca e verniz automotivo brilhante com detalhes de conjuntos com LEDs brancos, fio elétrico branco 2 x 0,5mm², na tensão de 220v. </t>
+  </si>
+  <si>
+    <t>Pastor e ovelha aramados, figuras tridimensionais, produzidas com arames de alumíno, pintura em epóxi na cor branca, aplicação de lâmpadas de LED brancas, com fio branco ou morno (medida do fio: 2x0,5mm²). Medidas das figuras: mínimo: Pastor 1,80 de altura x 0,60m de largura x 0,70m de comprimento e Ovelha  0,59m de altura x 0,17m de largura x 0,70m de comprimento  / máximo: Pastor 1,90m de altura x 0,70m de largura x 0,80m de comprimento e  Ovelha  0,49m de altura x 0,27m de largura x 0,80m de comprimento.</t>
   </si>
 </sst>
 </file>
@@ -562,7 +584,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Planilha4"/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
@@ -587,7 +609,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -596,7 +626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A254509-4FD2-42E1-AA3D-C634C34F4F17}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622607FC-FD87-41E1-A831-59A5C7EF8493}">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -605,43 +635,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -649,19 +679,109 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3072.29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2">
+        <f>C2*H2</f>
+        <v>9216.869999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A254509-4FD2-42E1-AA3D-C634C34F4F17}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
       </c>
       <c r="C2">
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
       </c>
       <c r="G2">
         <v>70</v>
@@ -673,13 +793,13 @@
         <v>10</v>
       </c>
       <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>32</v>
       </c>
       <c r="M2">
         <f>C2*H2</f>

</xml_diff>